<commit_message>
start eval on 128 dim autoencoder features
</commit_message>
<xml_diff>
--- a/eval/eval.xlsx
+++ b/eval/eval.xlsx
@@ -8,15 +8,50 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattchun/Documents/School/UW/cse547-final-project/eval/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D62068-27C8-2A47-937E-02ACFABD6F76}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673BB131-A245-C64F-AA98-D458F6907271}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="3460" windowWidth="16800" windowHeight="19520" activeTab="1" xr2:uid="{9CD26D36-3AD2-1A40-BD1C-ADCF605B4056}"/>
+    <workbookView xWindow="1320" yWindow="1320" windowWidth="29220" windowHeight="19520" activeTab="2" xr2:uid="{9CD26D36-3AD2-1A40-BD1C-ADCF605B4056}"/>
   </bookViews>
   <sheets>
     <sheet name="cb" sheetId="1" r:id="rId1"/>
-    <sheet name="graph cb" sheetId="2" r:id="rId2"/>
+    <sheet name="graph cb rmse" sheetId="2" r:id="rId2"/>
+    <sheet name="graph cb ILS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.16" hidden="1">'graph cb ILS'!$A$1</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'graph cb ILS'!$A$2:$A$21</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'graph cb ILS'!$B$1</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'graph cb ILS'!$B$2:$B$21</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'graph cb ILS'!$C$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'graph cb ILS'!$C$2:$C$21</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'graph cb ILS'!$D$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'graph cb ILS'!$D$2:$D$21</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'graph cb ILS'!$E$1</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'graph cb ILS'!$E$2:$E$21</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">'graph cb ILS'!$F$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">'graph cb ILS'!$F$2:$F$21</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">'graph cb ILS'!$G$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">'graph cb ILS'!$G$2:$G$21</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">'graph cb ILS'!$H$1</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">'graph cb ILS'!$H$2:$H$21</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">'graph cb ILS'!$A$1</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">'graph cb ILS'!$A$2:$A$21</definedName>
+    <definedName name="_xlchart.v2.10" hidden="1">'graph cb ILS'!$F$1</definedName>
+    <definedName name="_xlchart.v2.11" hidden="1">'graph cb ILS'!$F$2:$F$21</definedName>
+    <definedName name="_xlchart.v2.12" hidden="1">'graph cb ILS'!$G$1</definedName>
+    <definedName name="_xlchart.v2.13" hidden="1">'graph cb ILS'!$G$2:$G$21</definedName>
+    <definedName name="_xlchart.v2.14" hidden="1">'graph cb ILS'!$H$1</definedName>
+    <definedName name="_xlchart.v2.15" hidden="1">'graph cb ILS'!$H$2:$H$21</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">'graph cb ILS'!$B$1</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">'graph cb ILS'!$B$2:$B$21</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">'graph cb ILS'!$C$1</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">'graph cb ILS'!$C$2:$C$21</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">'graph cb ILS'!$D$1</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">'graph cb ILS'!$D$2:$D$21</definedName>
+    <definedName name="_xlchart.v2.8" hidden="1">'graph cb ILS'!$E$1</definedName>
+    <definedName name="_xlchart.v2.9" hidden="1">'graph cb ILS'!$E$2:$E$21</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>currK</t>
   </si>
@@ -59,6 +94,30 @@
   </si>
   <si>
     <t>rmse top 100</t>
+  </si>
+  <si>
+    <t>rmse Autoencoder</t>
+  </si>
+  <si>
+    <t>ILS top 5</t>
+  </si>
+  <si>
+    <t>ILS top 10</t>
+  </si>
+  <si>
+    <t>ILS top 15</t>
+  </si>
+  <si>
+    <t>ILS top 30</t>
+  </si>
+  <si>
+    <t>ILS top 50</t>
+  </si>
+  <si>
+    <t>ILS top 100</t>
+  </si>
+  <si>
+    <t>ILS Autoencoder</t>
   </si>
 </sst>
 </file>
@@ -136,6 +195,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800"/>
+              <a:t>k</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
+              <a:t> vs Average RMSE</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -149,7 +238,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -176,7 +265,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'graph cb'!$B$1</c:f>
+              <c:f>'graph cb rmse'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -199,7 +288,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'graph cb'!$A$2:$A$21</c:f>
+              <c:f>'graph cb rmse'!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -268,7 +357,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'graph cb'!$B$2:$B$21</c:f>
+              <c:f>'graph cb rmse'!$B$2:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -347,7 +436,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'graph cb'!$C$1</c:f>
+              <c:f>'graph cb rmse'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -370,7 +459,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'graph cb'!$A$2:$A$21</c:f>
+              <c:f>'graph cb rmse'!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -439,7 +528,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'graph cb'!$C$2:$C$21</c:f>
+              <c:f>'graph cb rmse'!$C$2:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -518,7 +607,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'graph cb'!$D$1</c:f>
+              <c:f>'graph cb rmse'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -541,7 +630,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'graph cb'!$A$2:$A$21</c:f>
+              <c:f>'graph cb rmse'!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -610,7 +699,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'graph cb'!$D$2:$D$21</c:f>
+              <c:f>'graph cb rmse'!$D$2:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -689,7 +778,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'graph cb'!$E$1</c:f>
+              <c:f>'graph cb rmse'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -712,7 +801,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'graph cb'!$A$2:$A$21</c:f>
+              <c:f>'graph cb rmse'!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -781,7 +870,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'graph cb'!$E$2:$E$21</c:f>
+              <c:f>'graph cb rmse'!$E$2:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -860,7 +949,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'graph cb'!$F$1</c:f>
+              <c:f>'graph cb rmse'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -883,7 +972,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'graph cb'!$A$2:$A$21</c:f>
+              <c:f>'graph cb rmse'!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -952,7 +1041,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'graph cb'!$F$2:$F$21</c:f>
+              <c:f>'graph cb rmse'!$F$2:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1031,7 +1120,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'graph cb'!$G$1</c:f>
+              <c:f>'graph cb rmse'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1054,7 +1143,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'graph cb'!$A$2:$A$21</c:f>
+              <c:f>'graph cb rmse'!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1123,7 +1212,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'graph cb'!$G$2:$G$21</c:f>
+              <c:f>'graph cb rmse'!$G$2:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1194,6 +1283,179 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-A66D-4F48-8107-09D17DBC98BA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'graph cb rmse'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rmse Autoencoder</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'graph cb rmse'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'graph cb rmse'!$H$2:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>7.9639397858535101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.98456357773789</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9909465437820604</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.1135498063990692</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.1295718242767201</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1336328334695303</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.1390373758453194</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.1506809242359193</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.1486858725158307</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.1497049174088101</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.1550943226420909</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.1604077999426501</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.1646229767788707</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.1704049048318197</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.1778299339974296</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.1834141454482108</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.1871442460836104</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.1935486444785592</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.1986220542060799</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.2019393406223902</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BF8A-704A-9D4E-EB8771ABFBEA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1216,6 +1478,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>k</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1238,7 +1555,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1264,7 +1581,7 @@
         <c:axId val="89468895"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="5"/>
+          <c:min val="6"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1282,6 +1599,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t> RMSE</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1298,7 +1675,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1340,7 +1717,1592 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>k vs Average ILS</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'graph cb ILS'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ILS top 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'graph cb ILS'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'graph cb ILS'!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>87.664704705263006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>86.544390610167</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92.923964812945002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>92.064677599305696</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>93.023164888694595</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>94.370575803644201</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>94.632209267726694</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>94.185946720392195</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>94.075177664367203</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>94.197405066700298</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>93.974609873305099</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>93.527778721335807</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>93.129375395865694</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>92.816169928066799</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>92.574623849474193</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>92.300170728077603</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>91.957021041317503</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>91.815909704121495</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>91.6777291414964</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>91.651477451576596</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-696C-134A-B910-BCE9FDEF9EFF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'graph cb ILS'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ILS top 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'graph cb ILS'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'graph cb ILS'!$C$2:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>89.717012008104902</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87.674756279006502</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.492096967408102</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89.297554311155906</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90.352124368762404</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.129153885555695</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90.398127977187897</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90.412520818981093</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90.299827031625298</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90.312818214215397</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>90.014752906299506</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>89.527905905239393</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>89.152450936618095</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>88.846108720069196</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>88.540554988015998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>88.174034678940899</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>87.833471240669596</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>87.618336820357499</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>87.4490545892547</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>87.284445823606802</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-696C-134A-B910-BCE9FDEF9EFF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'graph cb ILS'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ILS top 15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'graph cb ILS'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'graph cb ILS'!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>84.659734180595706</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78.041662013254395</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79.090561870739805</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>78.037422006636504</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>77.677597252765807</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>78.827543769183805</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>79.682623454277802</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80.097570312789202</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80.294858951358094</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>80.058177734634498</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>79.295278565624699</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>78.537283118554299</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>77.984173048732103</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>77.551752210696407</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>77.150960016500207</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>76.682591685115796</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>76.072310647513106</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>75.763537081950304</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>75.474066739745695</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>75.358646639038895</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-696C-134A-B910-BCE9FDEF9EFF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'graph cb ILS'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ILS top 30</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'graph cb ILS'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'graph cb ILS'!$E$2:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>74.189828905116798</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66.093943335987106</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69.023655284175007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65.855424044671693</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65.938509265234799</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66.664580558987794</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>67.388705128415396</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>68.066257057279202</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>68.124664355118995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>67.170189478607796</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>66.357657065935499</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65.505409591738299</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64.827267275113797</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>64.233103339274706</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>63.811969008917302</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>63.187495970563802</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>62.588446066118699</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>62.247900542857899</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>61.910938014194201</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>61.735415494037497</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-696C-134A-B910-BCE9FDEF9EFF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'graph cb ILS'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ILS top 50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'graph cb ILS'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'graph cb ILS'!$F$2:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>58.712516065507998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.711801532103699</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58.2945972945775</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57.982291861371799</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58.852214241283498</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.111202371521202</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61.576669212126603</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>62.702184612443197</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>62.356609880105601</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>61.825539391312802</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>61.5174378752045</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>61.173297847043102</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60.788596297114402</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>60.396166553750803</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60.165674294716297</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>59.802864883116001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>59.302459115269201</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>58.952440364145197</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>58.665641514892897</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>58.397133297824602</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-696C-134A-B910-BCE9FDEF9EFF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'graph cb ILS'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ILS top 100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'graph cb ILS'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'graph cb ILS'!$G$2:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>49.361951017332402</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49.792282578366702</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49.479336080816402</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49.316009261114402</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49.624558962523302</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50.0014086549917</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50.371253724369801</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50.677758020801697</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50.803301618646003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50.7698605596673</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.773577704168403</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50.741521289427702</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50.652310703640197</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50.548826467726599</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50.480288732654301</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>50.271349739699097</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50.143465683525903</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50.087302791206902</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>50.086610598622499</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>50.072021740981597</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-696C-134A-B910-BCE9FDEF9EFF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'graph cb ILS'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ILS Autoencoder</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'graph cb ILS'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'graph cb ILS'!$H$2:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>103.581628266362</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>103.811028409898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>103.928746913685</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>103.987727691358</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>104.04488972812599</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>104.058729121989</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>104.064213904835</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>104.072877271094</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>104.08603036586599</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>104.09372373489801</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>104.102526102903</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>104.107942507037</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>104.11125544137801</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>104.112783505306</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>104.11196753450101</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>104.10857061970999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>104.104164922942</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>104.09939625158199</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>104.095282659886</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>104.089948208347</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-696C-134A-B910-BCE9FDEF9EFF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1999150607"/>
+        <c:axId val="1999152287"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1999150607"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>k</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1999152287"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1999152287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="40"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Average ILS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1999150607"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1394,6 +3356,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1949,20 +3951,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1970,6 +4488,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56AA74A3-4E33-4242-8734-B1296C1A7E33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF2EC6C3-43A3-9042-A8F4-C3951F246FA4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3741,15 +6300,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D93E8EE-D257-BB40-8F65-FFA0B4C53D34}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="A1:G21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3771,8 +6330,11 @@
       <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3794,8 +6356,11 @@
       <c r="G2">
         <v>7.4446431202020298</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>7.9639397858535101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3817,8 +6382,11 @@
       <c r="G3">
         <v>7.0910752963432602</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>7.98456357773789</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <f>1+A3</f>
         <v>3</v>
@@ -3841,8 +6409,11 @@
       <c r="G4">
         <v>6.9771282085340101</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>7.9909465437820604</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" ref="A5:A20" si="0">1+A4</f>
         <v>4</v>
@@ -3865,8 +6436,11 @@
       <c r="G5">
         <v>6.8041632036425899</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>8.1135498063990692</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3889,8 +6463,11 @@
       <c r="G6">
         <v>6.7585172015775399</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>8.1295718242767201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3913,8 +6490,11 @@
       <c r="G7">
         <v>6.7380250639844901</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>8.1336328334695303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3937,8 +6517,11 @@
       <c r="G8">
         <v>6.6896401596915602</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>8.1390373758453194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3961,8 +6544,11 @@
       <c r="G9">
         <v>6.6339007838897599</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>8.1506809242359193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3985,8 +6571,11 @@
       <c r="G10">
         <v>6.56585667947411</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>8.1486858725158307</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -4009,8 +6598,11 @@
       <c r="G11">
         <v>6.5078383143373699</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11">
+        <v>8.1497049174088101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -4033,8 +6625,11 @@
       <c r="G12">
         <v>6.4633027672800001</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12">
+        <v>8.1550943226420909</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -4057,8 +6652,11 @@
       <c r="G13">
         <v>6.4167407456613503</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13">
+        <v>8.1604077999426501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -4081,8 +6679,11 @@
       <c r="G14">
         <v>6.3717853542956897</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14">
+        <v>8.1646229767788707</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -4105,8 +6706,11 @@
       <c r="G15">
         <v>6.3410054951543096</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <v>8.1704049048318197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -4129,8 +6733,11 @@
       <c r="G16">
         <v>6.3240949288581696</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16">
+        <v>8.1778299339974296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -4153,8 +6760,11 @@
       <c r="G17">
         <v>6.2962748050957797</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17">
+        <v>8.1834141454482108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -4177,8 +6787,11 @@
       <c r="G18">
         <v>6.2811983392249298</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18">
+        <v>8.1871442460836104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -4201,8 +6814,11 @@
       <c r="G19">
         <v>6.2826564867790298</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19">
+        <v>8.1935486444785592</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -4225,8 +6841,11 @@
       <c r="G20">
         <v>6.2965720927708801</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20">
+        <v>8.1986220542060799</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <f>1+A20</f>
         <v>20</v>
@@ -4248,6 +6867,589 @@
       </c>
       <c r="G21">
         <v>6.3098225104646604</v>
+      </c>
+      <c r="H21">
+        <v>8.2019393406223902</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109A8EEA-413B-E142-8012-FB656864D6BB}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>87.664704705263006</v>
+      </c>
+      <c r="C2">
+        <v>89.717012008104902</v>
+      </c>
+      <c r="D2">
+        <v>84.659734180595706</v>
+      </c>
+      <c r="E2">
+        <v>74.189828905116798</v>
+      </c>
+      <c r="F2">
+        <v>58.712516065507998</v>
+      </c>
+      <c r="G2">
+        <v>49.361951017332402</v>
+      </c>
+      <c r="H2">
+        <v>103.581628266362</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>86.544390610167</v>
+      </c>
+      <c r="C3">
+        <v>87.674756279006502</v>
+      </c>
+      <c r="D3">
+        <v>78.041662013254395</v>
+      </c>
+      <c r="E3">
+        <v>66.093943335987106</v>
+      </c>
+      <c r="F3">
+        <v>57.711801532103699</v>
+      </c>
+      <c r="G3">
+        <v>49.792282578366702</v>
+      </c>
+      <c r="H3">
+        <v>103.811028409898</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f>1+A3</f>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>92.923964812945002</v>
+      </c>
+      <c r="C4">
+        <v>90.492096967408102</v>
+      </c>
+      <c r="D4">
+        <v>79.090561870739805</v>
+      </c>
+      <c r="E4">
+        <v>69.023655284175007</v>
+      </c>
+      <c r="F4">
+        <v>58.2945972945775</v>
+      </c>
+      <c r="G4">
+        <v>49.479336080816402</v>
+      </c>
+      <c r="H4">
+        <v>103.928746913685</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f t="shared" ref="A5:A20" si="0">1+A4</f>
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>92.064677599305696</v>
+      </c>
+      <c r="C5">
+        <v>89.297554311155906</v>
+      </c>
+      <c r="D5">
+        <v>78.037422006636504</v>
+      </c>
+      <c r="E5">
+        <v>65.855424044671693</v>
+      </c>
+      <c r="F5">
+        <v>57.982291861371799</v>
+      </c>
+      <c r="G5">
+        <v>49.316009261114402</v>
+      </c>
+      <c r="H5">
+        <v>103.987727691358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>93.023164888694595</v>
+      </c>
+      <c r="C6">
+        <v>90.352124368762404</v>
+      </c>
+      <c r="D6">
+        <v>77.677597252765807</v>
+      </c>
+      <c r="E6">
+        <v>65.938509265234799</v>
+      </c>
+      <c r="F6">
+        <v>58.852214241283498</v>
+      </c>
+      <c r="G6">
+        <v>49.624558962523302</v>
+      </c>
+      <c r="H6">
+        <v>104.04488972812599</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>94.370575803644201</v>
+      </c>
+      <c r="C7">
+        <v>90.129153885555695</v>
+      </c>
+      <c r="D7">
+        <v>78.827543769183805</v>
+      </c>
+      <c r="E7">
+        <v>66.664580558987794</v>
+      </c>
+      <c r="F7">
+        <v>60.111202371521202</v>
+      </c>
+      <c r="G7">
+        <v>50.0014086549917</v>
+      </c>
+      <c r="H7">
+        <v>104.058729121989</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>94.632209267726694</v>
+      </c>
+      <c r="C8">
+        <v>90.398127977187897</v>
+      </c>
+      <c r="D8">
+        <v>79.682623454277802</v>
+      </c>
+      <c r="E8">
+        <v>67.388705128415396</v>
+      </c>
+      <c r="F8">
+        <v>61.576669212126603</v>
+      </c>
+      <c r="G8">
+        <v>50.371253724369801</v>
+      </c>
+      <c r="H8">
+        <v>104.064213904835</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>94.185946720392195</v>
+      </c>
+      <c r="C9">
+        <v>90.412520818981093</v>
+      </c>
+      <c r="D9">
+        <v>80.097570312789202</v>
+      </c>
+      <c r="E9">
+        <v>68.066257057279202</v>
+      </c>
+      <c r="F9">
+        <v>62.702184612443197</v>
+      </c>
+      <c r="G9">
+        <v>50.677758020801697</v>
+      </c>
+      <c r="H9">
+        <v>104.072877271094</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>94.075177664367203</v>
+      </c>
+      <c r="C10">
+        <v>90.299827031625298</v>
+      </c>
+      <c r="D10">
+        <v>80.294858951358094</v>
+      </c>
+      <c r="E10">
+        <v>68.124664355118995</v>
+      </c>
+      <c r="F10">
+        <v>62.356609880105601</v>
+      </c>
+      <c r="G10">
+        <v>50.803301618646003</v>
+      </c>
+      <c r="H10">
+        <v>104.08603036586599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>94.197405066700298</v>
+      </c>
+      <c r="C11">
+        <v>90.312818214215397</v>
+      </c>
+      <c r="D11">
+        <v>80.058177734634498</v>
+      </c>
+      <c r="E11">
+        <v>67.170189478607796</v>
+      </c>
+      <c r="F11">
+        <v>61.825539391312802</v>
+      </c>
+      <c r="G11">
+        <v>50.7698605596673</v>
+      </c>
+      <c r="H11">
+        <v>104.09372373489801</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>93.974609873305099</v>
+      </c>
+      <c r="C12">
+        <v>90.014752906299506</v>
+      </c>
+      <c r="D12">
+        <v>79.295278565624699</v>
+      </c>
+      <c r="E12">
+        <v>66.357657065935499</v>
+      </c>
+      <c r="F12">
+        <v>61.5174378752045</v>
+      </c>
+      <c r="G12">
+        <v>50.773577704168403</v>
+      </c>
+      <c r="H12">
+        <v>104.102526102903</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>93.527778721335807</v>
+      </c>
+      <c r="C13">
+        <v>89.527905905239393</v>
+      </c>
+      <c r="D13">
+        <v>78.537283118554299</v>
+      </c>
+      <c r="E13">
+        <v>65.505409591738299</v>
+      </c>
+      <c r="F13">
+        <v>61.173297847043102</v>
+      </c>
+      <c r="G13">
+        <v>50.741521289427702</v>
+      </c>
+      <c r="H13">
+        <v>104.107942507037</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>93.129375395865694</v>
+      </c>
+      <c r="C14">
+        <v>89.152450936618095</v>
+      </c>
+      <c r="D14">
+        <v>77.984173048732103</v>
+      </c>
+      <c r="E14">
+        <v>64.827267275113797</v>
+      </c>
+      <c r="F14">
+        <v>60.788596297114402</v>
+      </c>
+      <c r="G14">
+        <v>50.652310703640197</v>
+      </c>
+      <c r="H14">
+        <v>104.11125544137801</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>92.816169928066799</v>
+      </c>
+      <c r="C15">
+        <v>88.846108720069196</v>
+      </c>
+      <c r="D15">
+        <v>77.551752210696407</v>
+      </c>
+      <c r="E15">
+        <v>64.233103339274706</v>
+      </c>
+      <c r="F15">
+        <v>60.396166553750803</v>
+      </c>
+      <c r="G15">
+        <v>50.548826467726599</v>
+      </c>
+      <c r="H15">
+        <v>104.112783505306</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>92.574623849474193</v>
+      </c>
+      <c r="C16">
+        <v>88.540554988015998</v>
+      </c>
+      <c r="D16">
+        <v>77.150960016500207</v>
+      </c>
+      <c r="E16">
+        <v>63.811969008917302</v>
+      </c>
+      <c r="F16">
+        <v>60.165674294716297</v>
+      </c>
+      <c r="G16">
+        <v>50.480288732654301</v>
+      </c>
+      <c r="H16">
+        <v>104.11196753450101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>92.300170728077603</v>
+      </c>
+      <c r="C17">
+        <v>88.174034678940899</v>
+      </c>
+      <c r="D17">
+        <v>76.682591685115796</v>
+      </c>
+      <c r="E17">
+        <v>63.187495970563802</v>
+      </c>
+      <c r="F17">
+        <v>59.802864883116001</v>
+      </c>
+      <c r="G17">
+        <v>50.271349739699097</v>
+      </c>
+      <c r="H17">
+        <v>104.10857061970999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>91.957021041317503</v>
+      </c>
+      <c r="C18">
+        <v>87.833471240669596</v>
+      </c>
+      <c r="D18">
+        <v>76.072310647513106</v>
+      </c>
+      <c r="E18">
+        <v>62.588446066118699</v>
+      </c>
+      <c r="F18">
+        <v>59.302459115269201</v>
+      </c>
+      <c r="G18">
+        <v>50.143465683525903</v>
+      </c>
+      <c r="H18">
+        <v>104.104164922942</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>91.815909704121495</v>
+      </c>
+      <c r="C19">
+        <v>87.618336820357499</v>
+      </c>
+      <c r="D19">
+        <v>75.763537081950304</v>
+      </c>
+      <c r="E19">
+        <v>62.247900542857899</v>
+      </c>
+      <c r="F19">
+        <v>58.952440364145197</v>
+      </c>
+      <c r="G19">
+        <v>50.087302791206902</v>
+      </c>
+      <c r="H19">
+        <v>104.09939625158199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>91.6777291414964</v>
+      </c>
+      <c r="C20">
+        <v>87.4490545892547</v>
+      </c>
+      <c r="D20">
+        <v>75.474066739745695</v>
+      </c>
+      <c r="E20">
+        <v>61.910938014194201</v>
+      </c>
+      <c r="F20">
+        <v>58.665641514892897</v>
+      </c>
+      <c r="G20">
+        <v>50.086610598622499</v>
+      </c>
+      <c r="H20">
+        <v>104.095282659886</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f>1+A20</f>
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>91.651477451576596</v>
+      </c>
+      <c r="C21">
+        <v>87.284445823606802</v>
+      </c>
+      <c r="D21">
+        <v>75.358646639038895</v>
+      </c>
+      <c r="E21">
+        <v>61.735415494037497</v>
+      </c>
+      <c r="F21">
+        <v>58.397133297824602</v>
+      </c>
+      <c r="G21">
+        <v>50.072021740981597</v>
+      </c>
+      <c r="H21">
+        <v>104.089948208347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding most up to date eval spreadsheet
</commit_message>
<xml_diff>
--- a/eval/eval.xlsx
+++ b/eval/eval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattchun/Documents/School/UW/cse547-final-project/eval/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673BB131-A245-C64F-AA98-D458F6907271}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF931A20-98CB-CD4C-9D1F-1F30C2E476D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1320" windowWidth="29220" windowHeight="19520" activeTab="2" xr2:uid="{9CD26D36-3AD2-1A40-BD1C-ADCF605B4056}"/>
+    <workbookView xWindow="5540" yWindow="460" windowWidth="29020" windowHeight="22500" activeTab="2" xr2:uid="{9CD26D36-3AD2-1A40-BD1C-ADCF605B4056}"/>
   </bookViews>
   <sheets>
     <sheet name="cb" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>currK</t>
   </si>
@@ -96,9 +96,6 @@
     <t>rmse top 100</t>
   </si>
   <si>
-    <t>rmse Autoencoder</t>
-  </si>
-  <si>
     <t>ILS top 5</t>
   </si>
   <si>
@@ -117,7 +114,16 @@
     <t>ILS top 100</t>
   </si>
   <si>
-    <t>ILS Autoencoder</t>
+    <t>rmse Autoencoder 128</t>
+  </si>
+  <si>
+    <t>rmse Autoencoder 32</t>
+  </si>
+  <si>
+    <t>ILS Autoencoder 128</t>
+  </si>
+  <si>
+    <t>ILS Autoencoder 32</t>
   </si>
 </sst>
 </file>
@@ -1295,7 +1301,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>rmse Autoencoder</c:v>
+                  <c:v>rmse Autoencoder 32</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1456,6 +1462,179 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-BF8A-704A-9D4E-EB8771ABFBEA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'graph cb rmse'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rmse Autoencoder 128</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'graph cb rmse'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'graph cb rmse'!$I$2:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>7.9639397858535101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.98456357773789</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9909465437820604</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.1135498063990692</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.1295718242767201</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1336328334695303</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.1390373758453194</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.1506809242359193</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.1486858725158307</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.1497049174088101</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.1550943226420909</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.1604077999426501</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.1646229767788707</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.1704049048318197</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.1778299339974296</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.1834141454482108</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.1871442460836104</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.1935486444785592</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.1986220542060799</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.2019393406223902</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6EA0-A840-8336-0AFC308CCB1C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2885,7 +3064,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ILS Autoencoder</c:v>
+                  <c:v>ILS Autoencoder 32</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3046,6 +3225,179 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-696C-134A-B910-BCE9FDEF9EFF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'graph cb ILS'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ILS Autoencoder 128</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'graph cb ILS'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'graph cb ILS'!$I$2:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>103.581628266362</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>103.811028409898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>103.928746913685</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>103.987727691358</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>104.04488972812599</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>104.058729121989</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>104.064213904835</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>104.072877271094</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>104.08603036586599</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>104.09372373489801</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>104.102526102903</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>104.107942507037</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>104.11125544137801</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>104.112783505306</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>104.11196753450101</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>104.10857061970999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>104.104164922942</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>104.09939625158199</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>104.095282659886</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>104.089948208347</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-696C-134A-B910-BCE9FDEF9EFF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4471,16 +4823,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4512,15 +4864,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6300,15 +6652,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D93E8EE-D257-BB40-8F65-FFA0B4C53D34}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6331,10 +6683,13 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6359,8 +6714,11 @@
       <c r="H2">
         <v>7.9639397858535101</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>7.9639397858535101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6385,8 +6743,11 @@
       <c r="H3">
         <v>7.98456357773789</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>7.98456357773789</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <f>1+A3</f>
         <v>3</v>
@@ -6412,8 +6773,11 @@
       <c r="H4">
         <v>7.9909465437820604</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>7.9909465437820604</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" ref="A5:A20" si="0">1+A4</f>
         <v>4</v>
@@ -6439,8 +6803,11 @@
       <c r="H5">
         <v>8.1135498063990692</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>8.1135498063990692</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -6466,8 +6833,11 @@
       <c r="H6">
         <v>8.1295718242767201</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>8.1295718242767201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6493,8 +6863,11 @@
       <c r="H7">
         <v>8.1336328334695303</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <v>8.1336328334695303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6520,8 +6893,11 @@
       <c r="H8">
         <v>8.1390373758453194</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>8.1390373758453194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -6547,8 +6923,11 @@
       <c r="H9">
         <v>8.1506809242359193</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <v>8.1506809242359193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -6574,8 +6953,11 @@
       <c r="H10">
         <v>8.1486858725158307</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <v>8.1486858725158307</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -6601,8 +6983,11 @@
       <c r="H11">
         <v>8.1497049174088101</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <v>8.1497049174088101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -6628,8 +7013,11 @@
       <c r="H12">
         <v>8.1550943226420909</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <v>8.1550943226420909</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -6655,8 +7043,11 @@
       <c r="H13">
         <v>8.1604077999426501</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <v>8.1604077999426501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -6682,8 +7073,11 @@
       <c r="H14">
         <v>8.1646229767788707</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14">
+        <v>8.1646229767788707</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -6709,8 +7103,11 @@
       <c r="H15">
         <v>8.1704049048318197</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <v>8.1704049048318197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -6736,8 +7133,11 @@
       <c r="H16">
         <v>8.1778299339974296</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <v>8.1778299339974296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -6763,8 +7163,11 @@
       <c r="H17">
         <v>8.1834141454482108</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17">
+        <v>8.1834141454482108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -6790,8 +7193,11 @@
       <c r="H18">
         <v>8.1871442460836104</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18">
+        <v>8.1871442460836104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -6817,8 +7223,11 @@
       <c r="H19">
         <v>8.1935486444785592</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19">
+        <v>8.1935486444785592</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -6844,8 +7253,11 @@
       <c r="H20">
         <v>8.1986220542060799</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20">
+        <v>8.1986220542060799</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <f>1+A20</f>
         <v>20</v>
@@ -6869,6 +7281,9 @@
         <v>6.3098225104646604</v>
       </c>
       <c r="H21">
+        <v>8.2019393406223902</v>
+      </c>
+      <c r="I21">
         <v>8.2019393406223902</v>
       </c>
     </row>
@@ -6880,41 +7295,44 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109A8EEA-413B-E142-8012-FB656864D6BB}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6939,8 +7357,11 @@
       <c r="H2">
         <v>103.581628266362</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>103.581628266362</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6965,8 +7386,11 @@
       <c r="H3">
         <v>103.811028409898</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>103.811028409898</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <f>1+A3</f>
         <v>3</v>
@@ -6992,8 +7416,11 @@
       <c r="H4">
         <v>103.928746913685</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>103.928746913685</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" ref="A5:A20" si="0">1+A4</f>
         <v>4</v>
@@ -7019,8 +7446,11 @@
       <c r="H5">
         <v>103.987727691358</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>103.987727691358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -7046,8 +7476,11 @@
       <c r="H6">
         <v>104.04488972812599</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>104.04488972812599</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -7073,8 +7506,11 @@
       <c r="H7">
         <v>104.058729121989</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <v>104.058729121989</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -7100,8 +7536,11 @@
       <c r="H8">
         <v>104.064213904835</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>104.064213904835</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -7127,8 +7566,11 @@
       <c r="H9">
         <v>104.072877271094</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <v>104.072877271094</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -7154,8 +7596,11 @@
       <c r="H10">
         <v>104.08603036586599</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <v>104.08603036586599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -7181,8 +7626,11 @@
       <c r="H11">
         <v>104.09372373489801</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <v>104.09372373489801</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -7208,8 +7656,11 @@
       <c r="H12">
         <v>104.102526102903</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <v>104.102526102903</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -7235,8 +7686,11 @@
       <c r="H13">
         <v>104.107942507037</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <v>104.107942507037</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -7262,8 +7716,11 @@
       <c r="H14">
         <v>104.11125544137801</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14">
+        <v>104.11125544137801</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -7289,8 +7746,11 @@
       <c r="H15">
         <v>104.112783505306</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <v>104.112783505306</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -7316,8 +7776,11 @@
       <c r="H16">
         <v>104.11196753450101</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <v>104.11196753450101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -7343,8 +7806,11 @@
       <c r="H17">
         <v>104.10857061970999</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17">
+        <v>104.10857061970999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -7370,8 +7836,11 @@
       <c r="H18">
         <v>104.104164922942</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18">
+        <v>104.104164922942</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -7397,8 +7866,11 @@
       <c r="H19">
         <v>104.09939625158199</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19">
+        <v>104.09939625158199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -7424,8 +7896,11 @@
       <c r="H20">
         <v>104.095282659886</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20">
+        <v>104.095282659886</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <f>1+A20</f>
         <v>20</v>
@@ -7449,6 +7924,9 @@
         <v>50.072021740981597</v>
       </c>
       <c r="H21">
+        <v>104.089948208347</v>
+      </c>
+      <c r="I21">
         <v>104.089948208347</v>
       </c>
     </row>

</xml_diff>

<commit_message>
all the eval results
</commit_message>
<xml_diff>
--- a/eval/eval.xlsx
+++ b/eval/eval.xlsx
@@ -8,48 +8,57 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattchun/Documents/School/UW/cse547-final-project/eval/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF931A20-98CB-CD4C-9D1F-1F30C2E476D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16835C35-373C-8F41-8B37-2EB50490E7A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5540" yWindow="460" windowWidth="29020" windowHeight="22500" activeTab="2" xr2:uid="{9CD26D36-3AD2-1A40-BD1C-ADCF605B4056}"/>
+    <workbookView xWindow="5540" yWindow="460" windowWidth="29020" windowHeight="22500" activeTab="3" xr2:uid="{9CD26D36-3AD2-1A40-BD1C-ADCF605B4056}"/>
   </bookViews>
   <sheets>
     <sheet name="cb" sheetId="1" r:id="rId1"/>
     <sheet name="graph cb rmse" sheetId="2" r:id="rId2"/>
     <sheet name="graph cb ILS" sheetId="3" r:id="rId3"/>
+    <sheet name="hybrid rmse" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.16" hidden="1">'graph cb ILS'!$A$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'graph cb ILS'!$A$2:$A$21</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'graph cb ILS'!$B$1</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'graph cb ILS'!$B$2:$B$21</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'graph cb ILS'!$C$1</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'graph cb ILS'!$C$2:$C$21</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'graph cb ILS'!$D$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'graph cb ILS'!$D$2:$D$21</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">'graph cb ILS'!$E$1</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'graph cb ILS'!$E$2:$E$21</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">'graph cb ILS'!$F$1</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">'graph cb ILS'!$F$2:$F$21</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">'graph cb ILS'!$G$1</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">'graph cb ILS'!$G$2:$G$21</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">'graph cb ILS'!$H$1</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">'graph cb ILS'!$H$2:$H$21</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">'graph cb ILS'!$A$1</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">'graph cb ILS'!$A$2:$A$21</definedName>
-    <definedName name="_xlchart.v2.10" hidden="1">'graph cb ILS'!$F$1</definedName>
-    <definedName name="_xlchart.v2.11" hidden="1">'graph cb ILS'!$F$2:$F$21</definedName>
-    <definedName name="_xlchart.v2.12" hidden="1">'graph cb ILS'!$G$1</definedName>
-    <definedName name="_xlchart.v2.13" hidden="1">'graph cb ILS'!$G$2:$G$21</definedName>
-    <definedName name="_xlchart.v2.14" hidden="1">'graph cb ILS'!$H$1</definedName>
-    <definedName name="_xlchart.v2.15" hidden="1">'graph cb ILS'!$H$2:$H$21</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">'graph cb ILS'!$B$1</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">'graph cb ILS'!$B$2:$B$21</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">'graph cb ILS'!$C$1</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">'graph cb ILS'!$C$2:$C$21</definedName>
-    <definedName name="_xlchart.v2.6" hidden="1">'graph cb ILS'!$D$1</definedName>
-    <definedName name="_xlchart.v2.7" hidden="1">'graph cb ILS'!$D$2:$D$21</definedName>
-    <definedName name="_xlchart.v2.8" hidden="1">'graph cb ILS'!$E$1</definedName>
-    <definedName name="_xlchart.v2.9" hidden="1">'graph cb ILS'!$E$2:$E$21</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'hybrid rmse'!$A$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'hybrid rmse'!$A$2:$A$21</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'hybrid rmse'!$B$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'hybrid rmse'!$B$2:$B$21</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'hybrid rmse'!$C$1</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'hybrid rmse'!$C$2:$C$21</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">'hybrid rmse'!$D$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">'hybrid rmse'!$D$2:$D$21</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">'hybrid rmse'!$E$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">'hybrid rmse'!$E$2:$E$21</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">'hybrid rmse'!$F$1</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">'hybrid rmse'!$F$2:$F$21</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">'hybrid rmse'!$G$1</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">'hybrid rmse'!$G$2:$G$21</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">'hybrid rmse'!$H$1</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">'hybrid rmse'!$H$2:$H$21</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">'hybrid rmse'!$I$1</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">'hybrid rmse'!$I$2:$I$21</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">'hybrid rmse'!$J$1</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">'hybrid rmse'!$J$2:$J$21</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">'hybrid rmse'!$A$1</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">'hybrid rmse'!$A$2:$A$21</definedName>
+    <definedName name="_xlchart.v2.10" hidden="1">'hybrid rmse'!$F$1</definedName>
+    <definedName name="_xlchart.v2.11" hidden="1">'hybrid rmse'!$F$2:$F$21</definedName>
+    <definedName name="_xlchart.v2.12" hidden="1">'hybrid rmse'!$G$1</definedName>
+    <definedName name="_xlchart.v2.13" hidden="1">'hybrid rmse'!$G$2:$G$21</definedName>
+    <definedName name="_xlchart.v2.14" hidden="1">'hybrid rmse'!$H$1</definedName>
+    <definedName name="_xlchart.v2.15" hidden="1">'hybrid rmse'!$H$2:$H$21</definedName>
+    <definedName name="_xlchart.v2.16" hidden="1">'hybrid rmse'!$I$1</definedName>
+    <definedName name="_xlchart.v2.17" hidden="1">'hybrid rmse'!$I$2:$I$21</definedName>
+    <definedName name="_xlchart.v2.18" hidden="1">'hybrid rmse'!$J$1</definedName>
+    <definedName name="_xlchart.v2.19" hidden="1">'hybrid rmse'!$J$2:$J$21</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">'hybrid rmse'!$B$1</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">'hybrid rmse'!$B$2:$B$21</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">'hybrid rmse'!$C$1</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">'hybrid rmse'!$C$2:$C$21</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">'hybrid rmse'!$D$1</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">'hybrid rmse'!$D$2:$D$21</definedName>
+    <definedName name="_xlchart.v2.8" hidden="1">'hybrid rmse'!$E$1</definedName>
+    <definedName name="_xlchart.v2.9" hidden="1">'hybrid rmse'!$E$2:$E$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>currK</t>
   </si>
@@ -125,12 +134,39 @@
   <si>
     <t>ILS Autoencoder 32</t>
   </si>
+  <si>
+    <t>rmse hybrid top 5</t>
+  </si>
+  <si>
+    <t>rmse CF</t>
+  </si>
+  <si>
+    <t>rmse hybrid top 10</t>
+  </si>
+  <si>
+    <t>rmse hybrid top 15</t>
+  </si>
+  <si>
+    <t>rmse hybrid top 30</t>
+  </si>
+  <si>
+    <t>rmse hybrid top 50</t>
+  </si>
+  <si>
+    <t>rmse hybrid top 100</t>
+  </si>
+  <si>
+    <t>rmse hybrid Autoencoder 32</t>
+  </si>
+  <si>
+    <t>rmse hybrid Autoencoder 128</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -144,6 +180,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -166,9 +208,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3707,6 +3750,1942 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>k vs Average RMSE</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'hybrid rmse'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rmse hybrid top 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'hybrid rmse'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'hybrid rmse'!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>7.2853544110000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4128088339999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3922051480000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.2863807129999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3394020940000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3489332740000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.3188631700000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.2813830250000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.2528082439999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.2332096049999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.2150304600000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.1912722999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.1579397059999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.1364900359999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.1170244489999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.0875992700000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.0643992449999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.0425877469999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.023447108</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.9954140020000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BF8C-E64B-ADF2-AEB5C509D654}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'hybrid rmse'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rmse hybrid top 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'hybrid rmse'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'hybrid rmse'!$C$2:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>7.2723656200000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4282453850000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3533186500000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.2879894700000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3292839430000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3206623300000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.2810713500000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.2410225559999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.2089013560000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.1835769989999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.158513685</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.1338769309999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.1006063900000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.0736068249999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.0484743600000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.0082033890000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.9767639739999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.9457301710000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.9190055590000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.8871565419999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BF8C-E64B-ADF2-AEB5C509D654}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'hybrid rmse'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rmse hybrid top 15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'hybrid rmse'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'hybrid rmse'!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6.456184092</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.3445522370000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2566383290000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.2078249019999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.2317249779999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.2063055360000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1609058599999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.1061286109999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.0516999050000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.004137149</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.9607153339999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.91826103</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.8679670020000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.8297560080000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.7889619330000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.7349822990000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.688946917</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.6477567019999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.6109805670000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.5741596720000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BF8C-E64B-ADF2-AEB5C509D654}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'hybrid rmse'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rmse hybrid top 30</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'hybrid rmse'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'hybrid rmse'!$E$2:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6.3757440279999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.1715315759999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.1372443490000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0446987730000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.080181799</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0890328660000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0490565419999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.9951466489999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.9271503799999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.8691500650000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.819455971</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.7649910379999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.7101576319999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.6661938860000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.6151589819999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.5464214729999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.4822408779999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.4298241330000003</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.3834187419999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.3371130989999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-BF8C-E64B-ADF2-AEB5C509D654}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'hybrid rmse'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rmse hybrid top 50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'hybrid rmse'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'hybrid rmse'!$F$2:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6.4082751650000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2039147760000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.1936254569999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.1531381569999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.1765164800000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.1761529959999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1323026240000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.0740062449999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.0000503509999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.9234306339999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.8578280290000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.7952830239999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.7240017480000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.6648213470000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.6063105259999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.5287445960000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.4476692260000004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.3842439210000004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.3320137540000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.2788756899999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-BF8C-E64B-ADF2-AEB5C509D654}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'hybrid rmse'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rmse hybrid top 100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'hybrid rmse'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'hybrid rmse'!$G$2:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6.2388295569999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0413885389999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0043019769999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.9452267919999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.9673321049999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.9724902709999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.9235634319999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.8580716270000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.7725995130000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.6798954769999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.5982411399999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5088943070000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.4140065330000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.3306180579999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.2546452969999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.1615714319999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.0791964570000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.010813593</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.9563059589999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.8905468360000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-BF8C-E64B-ADF2-AEB5C509D654}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'hybrid rmse'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rmse hybrid Autoencoder 32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'hybrid rmse'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'hybrid rmse'!$H$2:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6.7958468300000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7565457279999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.7373721409999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.6248659249999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.5723870580000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.5492976860000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5523973900000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.5399452409999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.5407182800000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.5405074150000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.5618570329999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.5639918530000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.6098575390000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.6471219799999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.6632584960000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.6563859379999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.6655284889999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.6659573659999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.6670114099999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.6624596450000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-BF8C-E64B-ADF2-AEB5C509D654}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'hybrid rmse'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rmse hybrid Autoencoder 128</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'hybrid rmse'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'hybrid rmse'!$I$2:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6.7958468300000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7565457279999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.7373721409999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.6248659249999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.5723870580000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.5492976860000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5523973900000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.5399452409999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.5407182800000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.5405074150000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.5618570329999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.5639918530000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.6098575390000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.6471219799999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.6632584960000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.6563859379999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.6655284889999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.6659573659999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.6670114099999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.6624596450000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-BF8C-E64B-ADF2-AEB5C509D654}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'hybrid rmse'!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rmse CF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'hybrid rmse'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'hybrid rmse'!$J$2:$J$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>7.0410870660891103</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9360728805637297</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8641415608715297</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.8161119248741997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.7809870416933498</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.75367666089931</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.7257995453083499</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.7036765252392101</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.6867153862836801</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.6706771044127802</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.6606594340923202</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.6574833670598599</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.6516647050768496</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.6362927174530499</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.6320658618000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.6230966928688098</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.6197411996257101</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.6144661127572499</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.6082224194457497</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.60246663602629</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-BF8C-E64B-ADF2-AEB5C509D654}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1884571167"/>
+        <c:axId val="1884572847"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1884571167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:t>k</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1884572847"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1884572847"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="4.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Average RMSE</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1884571167"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3748,6 +5727,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4819,6 +6838,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4881,6 +7416,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF2EC6C3-43A3-9042-A8F4-C3951F246FA4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{653EE21D-A9C7-6E4F-8986-B2BE20C13D31}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6655,7 +9231,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7297,8 +9873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109A8EEA-413B-E142-8012-FB656864D6BB}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7934,4 +10510,1148 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0792A873-D924-E348-89EF-01D20ED184C2}">
+  <dimension ref="A1:M160"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>7.2853544110000001</v>
+      </c>
+      <c r="C2">
+        <v>7.2723656200000004</v>
+      </c>
+      <c r="D2">
+        <v>6.456184092</v>
+      </c>
+      <c r="E2">
+        <v>6.3757440279999997</v>
+      </c>
+      <c r="F2">
+        <v>6.4082751650000001</v>
+      </c>
+      <c r="G2">
+        <v>6.2388295569999999</v>
+      </c>
+      <c r="H2">
+        <v>6.7958468300000003</v>
+      </c>
+      <c r="I2">
+        <v>6.7958468300000003</v>
+      </c>
+      <c r="J2">
+        <v>7.0410870660891103</v>
+      </c>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>6.4128088339999998</v>
+      </c>
+      <c r="C3">
+        <v>6.4282453850000003</v>
+      </c>
+      <c r="D3">
+        <v>6.3445522370000003</v>
+      </c>
+      <c r="E3">
+        <v>6.1715315759999996</v>
+      </c>
+      <c r="F3">
+        <v>6.2039147760000004</v>
+      </c>
+      <c r="G3">
+        <v>6.0413885389999997</v>
+      </c>
+      <c r="H3">
+        <v>6.7565457279999999</v>
+      </c>
+      <c r="I3">
+        <v>6.7565457279999999</v>
+      </c>
+      <c r="J3">
+        <v>6.9360728805637297</v>
+      </c>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f>1+A3</f>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>6.3922051480000004</v>
+      </c>
+      <c r="C4">
+        <v>6.3533186500000003</v>
+      </c>
+      <c r="D4">
+        <v>6.2566383290000003</v>
+      </c>
+      <c r="E4">
+        <v>6.1372443490000004</v>
+      </c>
+      <c r="F4">
+        <v>6.1936254569999996</v>
+      </c>
+      <c r="G4">
+        <v>6.0043019769999999</v>
+      </c>
+      <c r="H4">
+        <v>6.7373721409999998</v>
+      </c>
+      <c r="I4">
+        <v>6.7373721409999998</v>
+      </c>
+      <c r="J4">
+        <v>6.8641415608715297</v>
+      </c>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f t="shared" ref="A5:A20" si="0">1+A4</f>
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>6.2863807129999998</v>
+      </c>
+      <c r="C5">
+        <v>6.2879894700000003</v>
+      </c>
+      <c r="D5">
+        <v>6.2078249019999996</v>
+      </c>
+      <c r="E5">
+        <v>6.0446987730000004</v>
+      </c>
+      <c r="F5">
+        <v>6.1531381569999999</v>
+      </c>
+      <c r="G5">
+        <v>5.9452267919999997</v>
+      </c>
+      <c r="H5">
+        <v>6.6248659249999999</v>
+      </c>
+      <c r="I5">
+        <v>6.6248659249999999</v>
+      </c>
+      <c r="J5">
+        <v>6.8161119248741997</v>
+      </c>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>6.3394020940000004</v>
+      </c>
+      <c r="C6">
+        <v>6.3292839430000001</v>
+      </c>
+      <c r="D6">
+        <v>6.2317249779999999</v>
+      </c>
+      <c r="E6">
+        <v>6.080181799</v>
+      </c>
+      <c r="F6">
+        <v>6.1765164800000001</v>
+      </c>
+      <c r="G6">
+        <v>5.9673321049999997</v>
+      </c>
+      <c r="H6">
+        <v>6.5723870580000003</v>
+      </c>
+      <c r="I6">
+        <v>6.5723870580000003</v>
+      </c>
+      <c r="J6">
+        <v>6.7809870416933498</v>
+      </c>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6.3489332740000002</v>
+      </c>
+      <c r="C7">
+        <v>6.3206623300000002</v>
+      </c>
+      <c r="D7">
+        <v>6.2063055360000003</v>
+      </c>
+      <c r="E7">
+        <v>6.0890328660000002</v>
+      </c>
+      <c r="F7">
+        <v>6.1761529959999999</v>
+      </c>
+      <c r="G7">
+        <v>5.9724902709999999</v>
+      </c>
+      <c r="H7">
+        <v>6.5492976860000001</v>
+      </c>
+      <c r="I7">
+        <v>6.5492976860000001</v>
+      </c>
+      <c r="J7">
+        <v>6.75367666089931</v>
+      </c>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>6.3188631700000002</v>
+      </c>
+      <c r="C8">
+        <v>6.2810713500000004</v>
+      </c>
+      <c r="D8">
+        <v>6.1609058599999997</v>
+      </c>
+      <c r="E8">
+        <v>6.0490565419999998</v>
+      </c>
+      <c r="F8">
+        <v>6.1323026240000003</v>
+      </c>
+      <c r="G8">
+        <v>5.9235634319999999</v>
+      </c>
+      <c r="H8">
+        <v>6.5523973900000003</v>
+      </c>
+      <c r="I8">
+        <v>6.5523973900000003</v>
+      </c>
+      <c r="J8">
+        <v>6.7257995453083499</v>
+      </c>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>6.2813830250000002</v>
+      </c>
+      <c r="C9">
+        <v>6.2410225559999999</v>
+      </c>
+      <c r="D9">
+        <v>6.1061286109999999</v>
+      </c>
+      <c r="E9">
+        <v>5.9951466489999996</v>
+      </c>
+      <c r="F9">
+        <v>6.0740062449999996</v>
+      </c>
+      <c r="G9">
+        <v>5.8580716270000002</v>
+      </c>
+      <c r="H9">
+        <v>6.5399452409999999</v>
+      </c>
+      <c r="I9">
+        <v>6.5399452409999999</v>
+      </c>
+      <c r="J9">
+        <v>6.7036765252392101</v>
+      </c>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>6.2528082439999997</v>
+      </c>
+      <c r="C10">
+        <v>6.2089013560000001</v>
+      </c>
+      <c r="D10">
+        <v>6.0516999050000004</v>
+      </c>
+      <c r="E10">
+        <v>5.9271503799999996</v>
+      </c>
+      <c r="F10">
+        <v>6.0000503509999996</v>
+      </c>
+      <c r="G10">
+        <v>5.7725995130000003</v>
+      </c>
+      <c r="H10">
+        <v>6.5407182800000001</v>
+      </c>
+      <c r="I10">
+        <v>6.5407182800000001</v>
+      </c>
+      <c r="J10">
+        <v>6.6867153862836801</v>
+      </c>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>6.2332096049999999</v>
+      </c>
+      <c r="C11">
+        <v>6.1835769989999996</v>
+      </c>
+      <c r="D11">
+        <v>6.004137149</v>
+      </c>
+      <c r="E11">
+        <v>5.8691500650000004</v>
+      </c>
+      <c r="F11">
+        <v>5.9234306339999998</v>
+      </c>
+      <c r="G11">
+        <v>5.6798954769999996</v>
+      </c>
+      <c r="H11">
+        <v>6.5405074150000004</v>
+      </c>
+      <c r="I11">
+        <v>6.5405074150000004</v>
+      </c>
+      <c r="J11">
+        <v>6.6706771044127802</v>
+      </c>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>6.2150304600000004</v>
+      </c>
+      <c r="C12">
+        <v>6.158513685</v>
+      </c>
+      <c r="D12">
+        <v>5.9607153339999996</v>
+      </c>
+      <c r="E12">
+        <v>5.819455971</v>
+      </c>
+      <c r="F12">
+        <v>5.8578280290000002</v>
+      </c>
+      <c r="G12">
+        <v>5.5982411399999998</v>
+      </c>
+      <c r="H12">
+        <v>6.5618570329999999</v>
+      </c>
+      <c r="I12">
+        <v>6.5618570329999999</v>
+      </c>
+      <c r="J12">
+        <v>6.6606594340923202</v>
+      </c>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>6.1912722999999996</v>
+      </c>
+      <c r="C13">
+        <v>6.1338769309999996</v>
+      </c>
+      <c r="D13">
+        <v>5.91826103</v>
+      </c>
+      <c r="E13">
+        <v>5.7649910379999998</v>
+      </c>
+      <c r="F13">
+        <v>5.7952830239999997</v>
+      </c>
+      <c r="G13">
+        <v>5.5088943070000003</v>
+      </c>
+      <c r="H13">
+        <v>6.5639918530000001</v>
+      </c>
+      <c r="I13">
+        <v>6.5639918530000001</v>
+      </c>
+      <c r="J13">
+        <v>6.6574833670598599</v>
+      </c>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>6.1579397059999996</v>
+      </c>
+      <c r="C14">
+        <v>6.1006063900000003</v>
+      </c>
+      <c r="D14">
+        <v>5.8679670020000003</v>
+      </c>
+      <c r="E14">
+        <v>5.7101576319999996</v>
+      </c>
+      <c r="F14">
+        <v>5.7240017480000001</v>
+      </c>
+      <c r="G14">
+        <v>5.4140065330000002</v>
+      </c>
+      <c r="H14">
+        <v>6.6098575390000001</v>
+      </c>
+      <c r="I14">
+        <v>6.6098575390000001</v>
+      </c>
+      <c r="J14">
+        <v>6.6516647050768496</v>
+      </c>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>6.1364900359999996</v>
+      </c>
+      <c r="C15">
+        <v>6.0736068249999997</v>
+      </c>
+      <c r="D15">
+        <v>5.8297560080000004</v>
+      </c>
+      <c r="E15">
+        <v>5.6661938860000003</v>
+      </c>
+      <c r="F15">
+        <v>5.6648213470000002</v>
+      </c>
+      <c r="G15">
+        <v>5.3306180579999998</v>
+      </c>
+      <c r="H15">
+        <v>6.6471219799999997</v>
+      </c>
+      <c r="I15">
+        <v>6.6471219799999997</v>
+      </c>
+      <c r="J15">
+        <v>6.6362927174530499</v>
+      </c>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>6.1170244489999996</v>
+      </c>
+      <c r="C16">
+        <v>6.0484743600000002</v>
+      </c>
+      <c r="D16">
+        <v>5.7889619330000004</v>
+      </c>
+      <c r="E16">
+        <v>5.6151589819999996</v>
+      </c>
+      <c r="F16">
+        <v>5.6063105259999997</v>
+      </c>
+      <c r="G16">
+        <v>5.2546452969999997</v>
+      </c>
+      <c r="H16">
+        <v>6.6632584960000001</v>
+      </c>
+      <c r="I16">
+        <v>6.6632584960000001</v>
+      </c>
+      <c r="J16">
+        <v>6.6320658618000001</v>
+      </c>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>6.0875992700000001</v>
+      </c>
+      <c r="C17">
+        <v>6.0082033890000002</v>
+      </c>
+      <c r="D17">
+        <v>5.7349822990000003</v>
+      </c>
+      <c r="E17">
+        <v>5.5464214729999997</v>
+      </c>
+      <c r="F17">
+        <v>5.5287445960000001</v>
+      </c>
+      <c r="G17">
+        <v>5.1615714319999997</v>
+      </c>
+      <c r="H17">
+        <v>6.6563859379999997</v>
+      </c>
+      <c r="I17">
+        <v>6.6563859379999997</v>
+      </c>
+      <c r="J17">
+        <v>6.6230966928688098</v>
+      </c>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>6.0643992449999997</v>
+      </c>
+      <c r="C18">
+        <v>5.9767639739999998</v>
+      </c>
+      <c r="D18">
+        <v>5.688946917</v>
+      </c>
+      <c r="E18">
+        <v>5.4822408779999998</v>
+      </c>
+      <c r="F18">
+        <v>5.4476692260000004</v>
+      </c>
+      <c r="G18">
+        <v>5.0791964570000001</v>
+      </c>
+      <c r="H18">
+        <v>6.6655284889999997</v>
+      </c>
+      <c r="I18">
+        <v>6.6655284889999997</v>
+      </c>
+      <c r="J18">
+        <v>6.6197411996257101</v>
+      </c>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>6.0425877469999998</v>
+      </c>
+      <c r="C19">
+        <v>5.9457301710000001</v>
+      </c>
+      <c r="D19">
+        <v>5.6477567019999997</v>
+      </c>
+      <c r="E19">
+        <v>5.4298241330000003</v>
+      </c>
+      <c r="F19">
+        <v>5.3842439210000004</v>
+      </c>
+      <c r="G19">
+        <v>5.010813593</v>
+      </c>
+      <c r="H19">
+        <v>6.6659573659999998</v>
+      </c>
+      <c r="I19">
+        <v>6.6659573659999998</v>
+      </c>
+      <c r="J19">
+        <v>6.6144661127572499</v>
+      </c>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>6.023447108</v>
+      </c>
+      <c r="C20">
+        <v>5.9190055590000004</v>
+      </c>
+      <c r="D20">
+        <v>5.6109805670000004</v>
+      </c>
+      <c r="E20">
+        <v>5.3834187419999999</v>
+      </c>
+      <c r="F20">
+        <v>5.3320137540000001</v>
+      </c>
+      <c r="G20">
+        <v>4.9563059589999998</v>
+      </c>
+      <c r="H20">
+        <v>6.6670114099999997</v>
+      </c>
+      <c r="I20">
+        <v>6.6670114099999997</v>
+      </c>
+      <c r="J20">
+        <v>6.6082224194457497</v>
+      </c>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f>1+A20</f>
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>5.9954140020000004</v>
+      </c>
+      <c r="C21">
+        <v>5.8871565419999996</v>
+      </c>
+      <c r="D21">
+        <v>5.5741596720000004</v>
+      </c>
+      <c r="E21">
+        <v>5.3371130989999997</v>
+      </c>
+      <c r="F21">
+        <v>5.2788756899999996</v>
+      </c>
+      <c r="G21">
+        <v>4.8905468360000004</v>
+      </c>
+      <c r="H21">
+        <v>6.6624596450000002</v>
+      </c>
+      <c r="I21">
+        <v>6.6624596450000002</v>
+      </c>
+      <c r="J21">
+        <v>6.60246663602629</v>
+      </c>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M33" s="2"/>
+    </row>
+    <row r="34" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M34" s="2"/>
+    </row>
+    <row r="35" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M35" s="2"/>
+    </row>
+    <row r="36" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M36" s="2"/>
+    </row>
+    <row r="37" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M37" s="2"/>
+    </row>
+    <row r="38" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M38" s="2"/>
+    </row>
+    <row r="39" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M39" s="2"/>
+    </row>
+    <row r="40" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M40" s="2"/>
+    </row>
+    <row r="41" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M41" s="2"/>
+    </row>
+    <row r="42" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M42" s="2"/>
+    </row>
+    <row r="43" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M43" s="2"/>
+    </row>
+    <row r="44" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M44" s="2"/>
+    </row>
+    <row r="45" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M45" s="2"/>
+    </row>
+    <row r="46" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M46" s="2"/>
+    </row>
+    <row r="47" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M47" s="2"/>
+    </row>
+    <row r="48" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M48" s="2"/>
+    </row>
+    <row r="49" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M49" s="2"/>
+    </row>
+    <row r="50" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M50" s="2"/>
+    </row>
+    <row r="51" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M51" s="2"/>
+    </row>
+    <row r="52" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M52" s="2"/>
+    </row>
+    <row r="53" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M53" s="2"/>
+    </row>
+    <row r="54" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M54" s="2"/>
+    </row>
+    <row r="55" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M55" s="2"/>
+    </row>
+    <row r="56" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M56" s="2"/>
+    </row>
+    <row r="57" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M57" s="2"/>
+    </row>
+    <row r="58" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M58" s="2"/>
+    </row>
+    <row r="59" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M59" s="2"/>
+    </row>
+    <row r="60" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M60" s="2"/>
+    </row>
+    <row r="61" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M61" s="2"/>
+    </row>
+    <row r="62" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M62" s="2"/>
+    </row>
+    <row r="63" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M63" s="2"/>
+    </row>
+    <row r="64" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M64" s="2"/>
+    </row>
+    <row r="65" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M65" s="2"/>
+    </row>
+    <row r="66" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M66" s="2"/>
+    </row>
+    <row r="67" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M67" s="2"/>
+    </row>
+    <row r="68" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M68" s="2"/>
+    </row>
+    <row r="69" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M69" s="2"/>
+    </row>
+    <row r="70" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M70" s="2"/>
+    </row>
+    <row r="71" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M71" s="2"/>
+    </row>
+    <row r="72" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M72" s="2"/>
+    </row>
+    <row r="73" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M73" s="2"/>
+    </row>
+    <row r="74" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M74" s="2"/>
+    </row>
+    <row r="75" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M75" s="2"/>
+    </row>
+    <row r="76" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M76" s="2"/>
+    </row>
+    <row r="77" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M77" s="2"/>
+    </row>
+    <row r="78" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M78" s="2"/>
+    </row>
+    <row r="79" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M79" s="2"/>
+    </row>
+    <row r="80" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M80" s="2"/>
+    </row>
+    <row r="81" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M81" s="2"/>
+    </row>
+    <row r="82" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M82" s="2"/>
+    </row>
+    <row r="83" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M83" s="2"/>
+    </row>
+    <row r="84" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M84" s="2"/>
+    </row>
+    <row r="85" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M85" s="2"/>
+    </row>
+    <row r="86" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M86" s="2"/>
+    </row>
+    <row r="87" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M87" s="2"/>
+    </row>
+    <row r="88" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M88" s="2"/>
+    </row>
+    <row r="89" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M89" s="2"/>
+    </row>
+    <row r="90" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M90" s="2"/>
+    </row>
+    <row r="91" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M91" s="2"/>
+    </row>
+    <row r="92" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M92" s="2"/>
+    </row>
+    <row r="93" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M93" s="2"/>
+    </row>
+    <row r="94" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M94" s="2"/>
+    </row>
+    <row r="95" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M95" s="2"/>
+    </row>
+    <row r="96" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M96" s="2"/>
+    </row>
+    <row r="97" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M97" s="2"/>
+    </row>
+    <row r="98" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M98" s="2"/>
+    </row>
+    <row r="99" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M99" s="2"/>
+    </row>
+    <row r="100" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M100" s="2"/>
+    </row>
+    <row r="101" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M101" s="2"/>
+    </row>
+    <row r="102" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M102" s="2"/>
+    </row>
+    <row r="103" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M103" s="2"/>
+    </row>
+    <row r="104" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M104" s="2"/>
+    </row>
+    <row r="105" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M105" s="2"/>
+    </row>
+    <row r="106" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M106" s="2"/>
+    </row>
+    <row r="107" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M107" s="2"/>
+    </row>
+    <row r="108" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M108" s="2"/>
+    </row>
+    <row r="109" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M109" s="2"/>
+    </row>
+    <row r="110" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M110" s="2"/>
+    </row>
+    <row r="111" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M111" s="2"/>
+    </row>
+    <row r="112" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M112" s="2"/>
+    </row>
+    <row r="113" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M113" s="2"/>
+    </row>
+    <row r="114" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M114" s="2"/>
+    </row>
+    <row r="115" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M115" s="2"/>
+    </row>
+    <row r="116" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M116" s="2"/>
+    </row>
+    <row r="117" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M117" s="2"/>
+    </row>
+    <row r="118" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M118" s="2"/>
+    </row>
+    <row r="119" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M119" s="2"/>
+    </row>
+    <row r="120" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M120" s="2"/>
+    </row>
+    <row r="121" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M121" s="2"/>
+    </row>
+    <row r="122" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M122" s="2"/>
+    </row>
+    <row r="123" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M123" s="2"/>
+    </row>
+    <row r="124" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M124" s="2"/>
+    </row>
+    <row r="125" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M125" s="2"/>
+    </row>
+    <row r="126" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M126" s="2"/>
+    </row>
+    <row r="127" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M127" s="2"/>
+    </row>
+    <row r="128" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M128" s="2"/>
+    </row>
+    <row r="129" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M129" s="2"/>
+    </row>
+    <row r="130" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M130" s="2"/>
+    </row>
+    <row r="131" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M131" s="2"/>
+    </row>
+    <row r="132" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M132" s="2"/>
+    </row>
+    <row r="133" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M133" s="2"/>
+    </row>
+    <row r="134" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M134" s="2"/>
+    </row>
+    <row r="135" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M135" s="2"/>
+    </row>
+    <row r="136" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M136" s="2"/>
+    </row>
+    <row r="137" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M137" s="2"/>
+    </row>
+    <row r="138" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M138" s="2"/>
+    </row>
+    <row r="139" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M139" s="2"/>
+    </row>
+    <row r="140" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M140" s="2"/>
+    </row>
+    <row r="141" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M141" s="2"/>
+    </row>
+    <row r="142" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M142" s="2"/>
+    </row>
+    <row r="143" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M143" s="2"/>
+    </row>
+    <row r="144" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M144" s="2"/>
+    </row>
+    <row r="145" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M145" s="2"/>
+    </row>
+    <row r="146" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M146" s="2"/>
+    </row>
+    <row r="147" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M147" s="2"/>
+    </row>
+    <row r="148" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M148" s="2"/>
+    </row>
+    <row r="149" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M149" s="2"/>
+    </row>
+    <row r="150" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M150" s="2"/>
+    </row>
+    <row r="151" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M151" s="2"/>
+    </row>
+    <row r="152" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M152" s="2"/>
+    </row>
+    <row r="153" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M153" s="2"/>
+    </row>
+    <row r="154" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M154" s="2"/>
+    </row>
+    <row r="155" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M155" s="2"/>
+    </row>
+    <row r="156" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M156" s="2"/>
+    </row>
+    <row r="157" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M157" s="2"/>
+    </row>
+    <row r="158" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M158" s="2"/>
+    </row>
+    <row r="159" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M159" s="2"/>
+    </row>
+    <row r="160" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M160" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>